<commit_message>
AJ: Testing: change of ActivitiesOverview.xlsx
</commit_message>
<xml_diff>
--- a/_data/ActivitiesOverview.xlsx
+++ b/_data/ActivitiesOverview.xlsx
@@ -157,7 +157,7 @@
     <t xml:space="preserve">MW</t>
   </si>
   <si>
-    <t xml:space="preserve">Fast fertig</t>
+    <t xml:space="preserve">Almost complete</t>
   </si>
   <si>
     <t xml:space="preserve">Pruning</t>
@@ -364,8 +364,8 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>